<commit_message>
Added comments or preferred label in column H; 'Outreach comments'
Sheena and Danica need to review.
</commit_message>
<xml_diff>
--- a/Load/ontology/harmonization/clinEpi_termWithMultipleLabelsWithSource.xlsx
+++ b/Load/ontology/harmonization/clinEpi_termWithMultipleLabelsWithSource.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10412"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiezheng/Documents/EuPathDB-git/ApiCommonData/Load/ontology/query_results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lindsabr\Desktop\Git\ApiCommonData\ApiCommonData\Load\ontology\harmonization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{E1A416F7-D48F-ED4A-8B99-1B6152326424}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85C7C439-2B7E-42A4-99FD-9A9C1D869102}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="980" windowWidth="20620" windowHeight="13680"/>
+    <workbookView xWindow="2031" yWindow="823" windowWidth="23255" windowHeight="14220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clinEpi_termWithMultipleLabelsW" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="190">
   <si>
     <t>sid</t>
   </si>
@@ -533,12 +533,69 @@
   </si>
   <si>
     <t>gates_scoreSeasonal</t>
+  </si>
+  <si>
+    <t>Outreach comments</t>
+  </si>
+  <si>
+    <t>Sheena &amp; Danica</t>
+  </si>
+  <si>
+    <t>Sheena</t>
+  </si>
+  <si>
+    <t>Remove ' seems like typo?</t>
+  </si>
+  <si>
+    <t>Agree</t>
+  </si>
+  <si>
+    <t>Case or control participant</t>
+  </si>
+  <si>
+    <t>Sheena &amp; Danica-rec two separate terms</t>
+  </si>
+  <si>
+    <t>Persistent diarrheal episode (more than 14 days)</t>
+  </si>
+  <si>
+    <t>Danica, why not just diet?</t>
+  </si>
+  <si>
+    <t>Sheena?</t>
+  </si>
+  <si>
+    <t>Recommend two different terms</t>
+  </si>
+  <si>
+    <t>Vesikari rehydration treatment</t>
+  </si>
+  <si>
+    <t>Drop variable</t>
+  </si>
+  <si>
+    <t>Oral poliovirus vaccine (OPV)</t>
+  </si>
+  <si>
+    <t>Inactivated poliovirus vaccine (IPV)</t>
+  </si>
+  <si>
+    <t>Last menstruation date available</t>
+  </si>
+  <si>
+    <t>Wasting severity</t>
+  </si>
+  <si>
+    <t>Stunting severity</t>
+  </si>
+  <si>
+    <t>Other illness</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1028,12 +1085,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1388,209 +1446,216 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C23" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
     <col min="3" max="3" width="77.5" customWidth="1"/>
     <col min="4" max="4" width="20.5" style="2" customWidth="1"/>
-    <col min="5" max="5" width="27.1640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="27.140625" style="2" customWidth="1"/>
     <col min="6" max="6" width="19" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="5" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="H1" s="5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" t="s">
+        <v>146</v>
+      </c>
+      <c r="H2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" t="s">
+        <v>146</v>
+      </c>
+      <c r="H3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" t="s">
+        <v>146</v>
+      </c>
+      <c r="H4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G5" t="s">
+        <v>146</v>
+      </c>
+      <c r="H5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G6" t="s">
+        <v>146</v>
+      </c>
+      <c r="H6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3">
-        <v>2</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="B7" s="3">
+        <v>2</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F7" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G7" s="3" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="3">
-        <v>2</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="B8" s="3">
+        <v>2</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E8" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F8" s="4" t="s">
         <v>127</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="3">
-        <v>2</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>122</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B9" s="3">
         <v>2</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>24</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>122</v>
@@ -1599,333 +1664,366 @@
         <v>133</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10">
-        <v>2</v>
-      </c>
-      <c r="C10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G10" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11">
-        <v>2</v>
-      </c>
-      <c r="C11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="3">
+        <v>2</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="3">
+        <v>2</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="H11" s="3"/>
+    </row>
+    <row r="12" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A12" s="3" t="s">
-        <v>33</v>
+        <v>86</v>
       </c>
       <c r="B12" s="3">
         <v>2</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>34</v>
+        <v>87</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>35</v>
+        <v>88</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>136</v>
+        <v>161</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13">
-        <v>2</v>
-      </c>
-      <c r="C13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="F13" s="2" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A13" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B13" s="3">
+        <v>2</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="H13" s="3"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A14" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B14" s="3">
+        <v>2</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="H14" s="3"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A15" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B15" s="3">
+        <v>2</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="H15" s="3"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A16" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B16" s="3">
+        <v>2</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="H16" s="3"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G17" t="s">
+        <v>141</v>
+      </c>
+      <c r="H17" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>77</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>78</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G18" t="s">
+        <v>159</v>
+      </c>
+      <c r="H18" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>67</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14">
-        <v>2</v>
-      </c>
-      <c r="C14" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="G14" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>41</v>
-      </c>
-      <c r="B15">
-        <v>2</v>
-      </c>
-      <c r="C15" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="F15" s="2" t="s">
+      <c r="G19" t="s">
+        <v>154</v>
+      </c>
+      <c r="H19" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>101</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>102</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="G15" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16">
-        <v>2</v>
-      </c>
-      <c r="C16" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="F16" s="2" t="s">
+      <c r="G20" t="s">
+        <v>167</v>
+      </c>
+      <c r="H20" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>104</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21" t="s">
+        <v>105</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>47</v>
-      </c>
-      <c r="B17">
-        <v>2</v>
-      </c>
-      <c r="C17" t="s">
-        <v>48</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G17" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>50</v>
-      </c>
-      <c r="B18">
-        <v>2</v>
-      </c>
-      <c r="C18" t="s">
-        <v>51</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="G18" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>53</v>
-      </c>
-      <c r="B19">
-        <v>2</v>
-      </c>
-      <c r="C19" t="s">
-        <v>54</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="G19" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>55</v>
-      </c>
-      <c r="B20">
-        <v>2</v>
-      </c>
-      <c r="C20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>58</v>
-      </c>
-      <c r="B21">
-        <v>2</v>
-      </c>
-      <c r="C21" t="s">
-        <v>59</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="F21" s="2" t="s">
+      <c r="G21" t="s">
+        <v>167</v>
+      </c>
+      <c r="H21" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>106</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22" t="s">
+        <v>107</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G22" t="s">
+        <v>182</v>
+      </c>
+      <c r="H22" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>109</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23" t="s">
+        <v>110</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G23" t="s">
+        <v>167</v>
+      </c>
+      <c r="H23" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>111</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24" t="s">
+        <v>112</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>61</v>
-      </c>
-      <c r="B22">
-        <v>2</v>
-      </c>
-      <c r="C22" t="s">
-        <v>62</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>64</v>
-      </c>
-      <c r="B23">
-        <v>2</v>
-      </c>
-      <c r="C23" t="s">
-        <v>65</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="G23" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>66</v>
-      </c>
-      <c r="B24">
-        <v>2</v>
-      </c>
-      <c r="C24" t="s">
-        <v>67</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>103</v>
-      </c>
       <c r="G24" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+        <v>167</v>
+      </c>
+      <c r="H24" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>68</v>
+        <v>113</v>
       </c>
       <c r="B25">
         <v>2</v>
       </c>
       <c r="C25" t="s">
-        <v>69</v>
+        <v>114</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="G25" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+        <v>167</v>
+      </c>
+      <c r="H25" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>71</v>
       </c>
@@ -1948,336 +2046,413 @@
         <v>157</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27" t="s">
+        <v>48</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G27" t="s">
+        <v>145</v>
+      </c>
+      <c r="H27" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G28" t="s">
+        <v>143</v>
+      </c>
+      <c r="H28" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>64</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29" t="s">
+        <v>65</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G29" t="s">
+        <v>143</v>
+      </c>
+      <c r="H29" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>68</v>
+      </c>
+      <c r="B30">
+        <v>2</v>
+      </c>
+      <c r="C30" t="s">
+        <v>69</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G30" t="s">
+        <v>143</v>
+      </c>
+      <c r="H30" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31">
+        <v>3</v>
+      </c>
+      <c r="C31" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="G31"/>
+      <c r="H31" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32">
+        <v>2</v>
+      </c>
+      <c r="C32" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="H32" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33">
+        <v>2</v>
+      </c>
+      <c r="C33" t="s">
+        <v>17</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="G33"/>
+      <c r="H33" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>19</v>
+      </c>
+      <c r="B34">
+        <v>2</v>
+      </c>
+      <c r="C34" t="s">
+        <v>20</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="G34"/>
+      <c r="H34" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>30</v>
+      </c>
+      <c r="B35">
+        <v>2</v>
+      </c>
+      <c r="C35" t="s">
+        <v>31</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="H35" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36">
+        <v>2</v>
+      </c>
+      <c r="C36" t="s">
+        <v>37</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H36" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37">
+        <v>2</v>
+      </c>
+      <c r="C37" t="s">
+        <v>45</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H37" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
+        <v>55</v>
+      </c>
+      <c r="B38">
+        <v>2</v>
+      </c>
+      <c r="C38" t="s">
+        <v>56</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="H38" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
+        <v>58</v>
+      </c>
+      <c r="B39">
+        <v>2</v>
+      </c>
+      <c r="C39" t="s">
+        <v>59</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H39" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A40" t="s">
+        <v>61</v>
+      </c>
+      <c r="B40">
+        <v>2</v>
+      </c>
+      <c r="C40" t="s">
+        <v>62</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="H40" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
         <v>74</v>
       </c>
-      <c r="B27">
-        <v>2</v>
-      </c>
-      <c r="C27" t="s">
+      <c r="B41">
+        <v>2</v>
+      </c>
+      <c r="C41" t="s">
         <v>75</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D41" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="E41" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="F41" s="2" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>77</v>
-      </c>
-      <c r="B28">
-        <v>2</v>
-      </c>
-      <c r="C28" t="s">
-        <v>78</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="G28" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+      <c r="H41" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A42" t="s">
         <v>80</v>
       </c>
-      <c r="B29">
-        <v>2</v>
-      </c>
-      <c r="C29" t="s">
+      <c r="B42">
+        <v>2</v>
+      </c>
+      <c r="C42" t="s">
         <v>81</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D42" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="E42" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="F42" s="2" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>83</v>
-      </c>
-      <c r="B30">
-        <v>2</v>
-      </c>
-      <c r="C30" t="s">
-        <v>84</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="G30" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="B31" s="3">
-        <v>2</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>89</v>
-      </c>
-      <c r="B32">
-        <v>2</v>
-      </c>
-      <c r="C32" t="s">
-        <v>90</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="G32" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B33" s="3">
-        <v>2</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B34" s="3">
-        <v>2</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+      <c r="G42"/>
+      <c r="H42" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A43" t="s">
         <v>98</v>
       </c>
-      <c r="B35">
-        <v>2</v>
-      </c>
-      <c r="C35" t="s">
+      <c r="B43">
+        <v>2</v>
+      </c>
+      <c r="C43" t="s">
         <v>99</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D43" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="E43" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="F35" s="2" t="s">
+      <c r="F43" s="2" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>101</v>
-      </c>
-      <c r="B36">
-        <v>2</v>
-      </c>
-      <c r="C36" t="s">
-        <v>102</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="G36" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>104</v>
-      </c>
-      <c r="B37">
-        <v>2</v>
-      </c>
-      <c r="C37" t="s">
-        <v>105</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="G37" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>106</v>
-      </c>
-      <c r="B38">
-        <v>2</v>
-      </c>
-      <c r="C38" t="s">
-        <v>107</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="G38" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>109</v>
-      </c>
-      <c r="B39">
-        <v>2</v>
-      </c>
-      <c r="C39" t="s">
-        <v>110</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="G39" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>111</v>
-      </c>
-      <c r="B40">
-        <v>2</v>
-      </c>
-      <c r="C40" t="s">
-        <v>112</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="G40" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>113</v>
-      </c>
-      <c r="B41">
-        <v>2</v>
-      </c>
-      <c r="C41" t="s">
-        <v>114</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="G41" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="B42" s="3">
-        <v>2</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="E42" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="F42" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="G42" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="B43" s="3">
-        <v>2</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="E43" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="F43" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="G43" s="3" t="s">
-        <v>133</v>
+      <c r="G43"/>
+      <c r="H43" t="s">
+        <v>183</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H43">
+    <sortCondition ref="G2:G43"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
label harmonization per redmine #39901
comments added to .xlsx file
</commit_message>
<xml_diff>
--- a/Load/ontology/harmonization/clinEpi_termWithMultipleLabelsWithSource.xlsx
+++ b/Load/ontology/harmonization/clinEpi_termWithMultipleLabelsWithSource.xlsx
@@ -1,26 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dhelb/Documents/GitHub/ApiCommonData/Load/ontology/harmonization/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jjudkins/Documents/GitHub/ApiCommonData/Load/ontology/harmonization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2705C035-0034-6E4D-8CCA-5CDDADA49417}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF78E95E-FBC3-544C-9862-51BBFF1374C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clinEpi_termWithMultipleLabelsW" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="208">
   <si>
     <t>sid</t>
   </si>
@@ -623,6 +633,27 @@
   </si>
   <si>
     <t>Test result summary for stool</t>
+  </si>
+  <si>
+    <t>JJ commments</t>
+  </si>
+  <si>
+    <t>changed all to 'Days vomiting'</t>
+  </si>
+  <si>
+    <t>dropped</t>
+  </si>
+  <si>
+    <t>EUPATH:0040021 for 'Antimalarial treatment prescribed'</t>
+  </si>
+  <si>
+    <t>new IRI: EUPATH:0040022</t>
+  </si>
+  <si>
+    <t>fixed. Using HP:0003418 for 'Back pain'</t>
+  </si>
+  <si>
+    <t>fixed. Using EUPATH:0022268 for 'Malaria…'</t>
   </si>
 </sst>
 </file>
@@ -1498,12 +1529,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
+      <selection pane="bottomLeft" activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1516,9 +1547,10 @@
     <col min="6" max="6" width="19" style="5" customWidth="1"/>
     <col min="7" max="7" width="31" style="4" customWidth="1"/>
     <col min="8" max="8" width="30.83203125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1543,8 +1575,11 @@
       <c r="H1" s="3" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" s="1" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="I1" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="1" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>27</v>
       </c>
@@ -1565,8 +1600,11 @@
       <c r="H2" s="4" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="I2" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>50</v>
       </c>
@@ -1585,8 +1623,11 @@
       <c r="H3" s="4" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" s="1" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="I3" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="1" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>53</v>
       </c>
@@ -1607,8 +1648,11 @@
       <c r="H4" s="4" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="I4" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>83</v>
       </c>
@@ -1627,8 +1671,11 @@
       <c r="H5" s="4" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="I5" s="4" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>89</v>
       </c>
@@ -1647,8 +1694,11 @@
       <c r="H6" s="4" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="85" x14ac:dyDescent="0.2">
+      <c r="I6" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="85" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
@@ -1672,7 +1722,7 @@
       </c>
       <c r="H7" s="6"/>
     </row>
-    <row r="8" spans="1:8" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>10</v>
       </c>
@@ -1696,7 +1746,7 @@
       </c>
       <c r="H8" s="6"/>
     </row>
-    <row r="9" spans="1:8" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>22</v>
       </c>
@@ -1720,7 +1770,7 @@
       </c>
       <c r="H9" s="6"/>
     </row>
-    <row r="10" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>25</v>
       </c>
@@ -1744,7 +1794,7 @@
       </c>
       <c r="H10" s="6"/>
     </row>
-    <row r="11" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>33</v>
       </c>
@@ -1768,7 +1818,7 @@
       </c>
       <c r="H11" s="6"/>
     </row>
-    <row r="12" spans="1:8" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>86</v>
       </c>
@@ -1792,7 +1842,7 @@
       </c>
       <c r="H12" s="6"/>
     </row>
-    <row r="13" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>92</v>
       </c>
@@ -1816,7 +1866,7 @@
       </c>
       <c r="H13" s="6"/>
     </row>
-    <row r="14" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>95</v>
       </c>
@@ -1840,7 +1890,7 @@
       </c>
       <c r="H14" s="6"/>
     </row>
-    <row r="15" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>115</v>
       </c>
@@ -1864,7 +1914,7 @@
       </c>
       <c r="H15" s="6"/>
     </row>
-    <row r="16" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>118</v>
       </c>
@@ -1888,7 +1938,7 @@
       </c>
       <c r="H16" s="6"/>
     </row>
-    <row r="17" spans="1:8" ht="68" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="68" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>38</v>
       </c>
@@ -1913,8 +1963,11 @@
       <c r="H17" s="9" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="I17" s="9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>77</v>
       </c>
@@ -1933,8 +1986,11 @@
       <c r="H18" s="4" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="I18" s="4" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>66</v>
       </c>
@@ -1959,8 +2015,11 @@
       <c r="H19" s="4" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="I19" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>101</v>
       </c>
@@ -1979,8 +2038,11 @@
       <c r="H20" s="4" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="I20" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>104</v>
       </c>
@@ -1999,8 +2061,11 @@
       <c r="H21" s="4" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="I21" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>106</v>
       </c>
@@ -2019,8 +2084,11 @@
       <c r="H22" s="4" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="I22" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>109</v>
       </c>
@@ -2039,8 +2107,11 @@
       <c r="H23" s="4" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="I23" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>111</v>
       </c>
@@ -2060,7 +2131,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>113</v>
       </c>
@@ -2079,8 +2150,11 @@
       <c r="H25" s="4" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="I25" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>71</v>
       </c>
@@ -2105,8 +2179,11 @@
       <c r="H26" s="4" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" ht="68" x14ac:dyDescent="0.2">
+      <c r="I26" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="68" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>47</v>
       </c>
@@ -2125,8 +2202,11 @@
       <c r="H27" s="4" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="I27" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>41</v>
       </c>
@@ -2151,8 +2231,11 @@
       <c r="H28" s="5" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="I28" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>64</v>
       </c>
@@ -2177,8 +2260,11 @@
       <c r="H29" s="4" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="I29" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>68</v>
       </c>
@@ -2203,8 +2289,11 @@
       <c r="H30" s="4" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" s="1" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="I30" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" s="1" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>7</v>
       </c>
@@ -2227,8 +2316,11 @@
       <c r="H31" s="4" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="I31" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>13</v>
       </c>
@@ -2250,8 +2342,11 @@
       <c r="H32" s="4" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="I32" s="4" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>16</v>
       </c>
@@ -2274,8 +2369,11 @@
       <c r="H33" s="6" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="I33" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>19</v>
       </c>
@@ -2298,8 +2396,11 @@
       <c r="H34" s="6" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="I34" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>30</v>
       </c>
@@ -2321,8 +2422,11 @@
       <c r="H35" s="6" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="I35" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>36</v>
       </c>
@@ -2344,8 +2448,11 @@
       <c r="H36" s="4" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="I36" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>44</v>
       </c>
@@ -2367,8 +2474,11 @@
       <c r="H37" s="4" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="I37" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>55</v>
       </c>
@@ -2390,8 +2500,11 @@
       <c r="H38" s="4" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="I38" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>58</v>
       </c>
@@ -2413,8 +2526,11 @@
       <c r="H39" s="4" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="I39" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>61</v>
       </c>
@@ -2436,8 +2552,11 @@
       <c r="H40" s="4" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="I40" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>74</v>
       </c>
@@ -2459,8 +2578,11 @@
       <c r="H41" s="4" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="I41" s="4" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>80</v>
       </c>
@@ -2483,8 +2605,11 @@
       <c r="H42" s="4" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="I42" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>98</v>
       </c>
@@ -2507,9 +2632,12 @@
       <c r="H43" s="4" t="s">
         <v>177</v>
       </c>
+      <c r="I43" s="1" t="s">
+        <v>203</v>
+      </c>
     </row>
   </sheetData>
-  <sortState ref="A2:H43">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H43">
     <sortCondition ref="G2:G43"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>